<commit_message>
1/16 diary added --Weihuan Fu
</commit_message>
<xml_diff>
--- a/diaries/diary-weihuan-fu.xlsx
+++ b/diaries/diary-weihuan-fu.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weihuanfu/Documents/MSWE/Winter 2020/SWE 265P/W2020/diaries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weihuanfu/Documents/MSWE/Winter 2020/SWE 265P/Diary/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602FF25F-29AD-FE47-A837-FCC4DFD338CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D526EB89-97F1-7047-A99D-11EEF0FDB4B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -54,39 +54,18 @@
     <t>Participants</t>
   </si>
   <si>
-    <t>&lt;what day?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;what time?&gt;</t>
-  </si>
-  <si>
     <t>Reflection</t>
   </si>
   <si>
-    <t>&lt;as applicable, with whom?&gt;</t>
-  </si>
-  <si>
     <t>Your Overall Mood</t>
   </si>
   <si>
     <t>Goal</t>
   </si>
   <si>
-    <t>&lt;what did you want to accomplish?&gt;</t>
-  </si>
-  <si>
     <t>Achievements</t>
   </si>
   <si>
-    <t>&lt;what did you actually accomplish?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;what insight(s) did you gain?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;how did you feel during the activity?&gt;</t>
-  </si>
-  <si>
     <t>Etc.</t>
   </si>
   <si>
@@ -108,9 +87,6 @@
     <t>cloned class repo to local directory</t>
   </si>
   <si>
-    <t xml:space="preserve">better understand how collaborative git is  </t>
-  </si>
-  <si>
     <t>Excited to work on open source project for the future</t>
   </si>
   <si>
@@ -120,10 +96,31 @@
     <t>Downlaod two open source project and get them running on local IDE</t>
   </si>
   <si>
-    <t>excited for collaborative work on the same project</t>
-  </si>
-  <si>
     <t>Myself</t>
+  </si>
+  <si>
+    <t>class time</t>
+  </si>
+  <si>
+    <t>understand and practice how to precisely locate issues that needs to be fixed in a system with a bunch of codes and classes</t>
+  </si>
+  <si>
+    <t>Ended up having to use a Git GUI App called Fork for cloning, committing, pushing and create merge request. Much easier than use git command line functions to manipulate version control locally</t>
+  </si>
+  <si>
+    <t>understand the importance of version control especially when everyone if working on different parts of one system. Got familiar with the basic functions of git GUI but more terms need to be learned in the future such as how to deal with merge conflict</t>
+  </si>
+  <si>
+    <t>excited to learn something that is widely used in the industry.</t>
+  </si>
+  <si>
+    <t>learned and practiced multiple theories of how to locate issues. Leaned about some common ways of naming files such as "sprite". Learn the way of approaching and finally locate the code we want to change</t>
+  </si>
+  <si>
+    <t>It is hard to understand every line of code in a big system but it is almost unnecessary to be able to do so (because everyone usually has their own modules), however it is very useful to understand how the majority functions works in terms of the software behavior. And being able to quickly do so, locate problem and fix it will be very efficient</t>
+  </si>
+  <si>
+    <t>Not really familiar with reading codes that are writtened by others but excited to learn a lot from reading other people code.</t>
   </si>
 </sst>
 </file>
@@ -246,12 +243,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -262,7 +274,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -288,16 +300,25 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="9" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -621,33 +642,38 @@
   <dimension ref="A1:G125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="7" width="34.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="4" width="42.83203125" customWidth="1"/>
+    <col min="5" max="5" width="41.5" customWidth="1"/>
+    <col min="6" max="7" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -663,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -675,8 +701,8 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>21</v>
+      <c r="B5" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -689,7 +715,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -716,107 +742,107 @@
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="12">
+        <v>43839</v>
+      </c>
+      <c r="B10" s="13">
+        <v>0.875</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="6" t="s">
+      <c r="D10" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="A11" s="12">
+        <v>43842</v>
+      </c>
+      <c r="B11" s="13">
+        <v>0.47361111111111115</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+      <c r="A12" s="12">
+        <v>43846</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
-        <v>43839</v>
-      </c>
-      <c r="B10" s="10">
-        <v>0.875</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="9">
-        <v>43842</v>
-      </c>
-      <c r="B11" s="10">
-        <v>0.47361111111111115</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="15"/>
     </row>
     <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>

</xml_diff>

<commit_message>
1/16 diary added --Weihuan Fu (#61)
</commit_message>
<xml_diff>
--- a/diaries/diary-weihuan-fu.xlsx
+++ b/diaries/diary-weihuan-fu.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weihuanfu/Documents/MSWE/Winter 2020/SWE 265P/W2020/diaries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weihuanfu/Documents/MSWE/Winter 2020/SWE 265P/Diary/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602FF25F-29AD-FE47-A837-FCC4DFD338CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D526EB89-97F1-7047-A99D-11EEF0FDB4B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -54,39 +54,18 @@
     <t>Participants</t>
   </si>
   <si>
-    <t>&lt;what day?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;what time?&gt;</t>
-  </si>
-  <si>
     <t>Reflection</t>
   </si>
   <si>
-    <t>&lt;as applicable, with whom?&gt;</t>
-  </si>
-  <si>
     <t>Your Overall Mood</t>
   </si>
   <si>
     <t>Goal</t>
   </si>
   <si>
-    <t>&lt;what did you want to accomplish?&gt;</t>
-  </si>
-  <si>
     <t>Achievements</t>
   </si>
   <si>
-    <t>&lt;what did you actually accomplish?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;what insight(s) did you gain?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;how did you feel during the activity?&gt;</t>
-  </si>
-  <si>
     <t>Etc.</t>
   </si>
   <si>
@@ -108,9 +87,6 @@
     <t>cloned class repo to local directory</t>
   </si>
   <si>
-    <t xml:space="preserve">better understand how collaborative git is  </t>
-  </si>
-  <si>
     <t>Excited to work on open source project for the future</t>
   </si>
   <si>
@@ -120,10 +96,31 @@
     <t>Downlaod two open source project and get them running on local IDE</t>
   </si>
   <si>
-    <t>excited for collaborative work on the same project</t>
-  </si>
-  <si>
     <t>Myself</t>
+  </si>
+  <si>
+    <t>class time</t>
+  </si>
+  <si>
+    <t>understand and practice how to precisely locate issues that needs to be fixed in a system with a bunch of codes and classes</t>
+  </si>
+  <si>
+    <t>Ended up having to use a Git GUI App called Fork for cloning, committing, pushing and create merge request. Much easier than use git command line functions to manipulate version control locally</t>
+  </si>
+  <si>
+    <t>understand the importance of version control especially when everyone if working on different parts of one system. Got familiar with the basic functions of git GUI but more terms need to be learned in the future such as how to deal with merge conflict</t>
+  </si>
+  <si>
+    <t>excited to learn something that is widely used in the industry.</t>
+  </si>
+  <si>
+    <t>learned and practiced multiple theories of how to locate issues. Leaned about some common ways of naming files such as "sprite". Learn the way of approaching and finally locate the code we want to change</t>
+  </si>
+  <si>
+    <t>It is hard to understand every line of code in a big system but it is almost unnecessary to be able to do so (because everyone usually has their own modules), however it is very useful to understand how the majority functions works in terms of the software behavior. And being able to quickly do so, locate problem and fix it will be very efficient</t>
+  </si>
+  <si>
+    <t>Not really familiar with reading codes that are writtened by others but excited to learn a lot from reading other people code.</t>
   </si>
 </sst>
 </file>
@@ -246,12 +243,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -262,7 +274,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -288,16 +300,25 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="9" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -621,33 +642,38 @@
   <dimension ref="A1:G125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="7" width="34.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="4" width="42.83203125" customWidth="1"/>
+    <col min="5" max="5" width="41.5" customWidth="1"/>
+    <col min="6" max="7" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -663,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -675,8 +701,8 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>21</v>
+      <c r="B5" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -689,7 +715,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -716,107 +742,107 @@
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="12">
+        <v>43839</v>
+      </c>
+      <c r="B10" s="13">
+        <v>0.875</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="6" t="s">
+      <c r="D10" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="A11" s="12">
+        <v>43842</v>
+      </c>
+      <c r="B11" s="13">
+        <v>0.47361111111111115</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+      <c r="A12" s="12">
+        <v>43846</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
-        <v>43839</v>
-      </c>
-      <c r="B10" s="10">
-        <v>0.875</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="9">
-        <v>43842</v>
-      </c>
-      <c r="B11" s="10">
-        <v>0.47361111111111115</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="15"/>
     </row>
     <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>

</xml_diff>

<commit_message>
2 diaries added -- Weihuan Fu
</commit_message>
<xml_diff>
--- a/diaries/diary-weihuan-fu.xlsx
+++ b/diaries/diary-weihuan-fu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weihuanfu/Desktop/SWE-265P/Diary/diaries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6769CD-EE20-2949-AFDC-104462E665BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8B97EF-F55E-48E0-A6FA-9CD2A599FFA3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="77">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -245,6 +245,36 @@
   </si>
   <si>
     <t>good because the homework is finished</t>
+  </si>
+  <si>
+    <t>classtime</t>
+  </si>
+  <si>
+    <t>learn more about how mental model works and how to practice on it. Get career insights from guest speaker</t>
+  </si>
+  <si>
+    <t>feel lucky talking with somewho who's been writing codes for most of his life</t>
+  </si>
+  <si>
+    <t>Almost the only way to improve coding skills is to keep reading codes from either yourself that you wrote years ago, or from others, and delibrately practice by writing a lot of codes. Meanwhile, while it is suggested to schedule a chunk of time just sit there and dive into codes, it is better to take small breaks as well to avoid burn out.</t>
+  </si>
+  <si>
+    <t>Learned about how midterm will be like and what kind of questions will be on the midterm</t>
+  </si>
+  <si>
+    <t>self</t>
+  </si>
+  <si>
+    <t>review midterm</t>
+  </si>
+  <si>
+    <t>made a study plan as well as all important notes of concepts and practice convered so far, will go into more details tmr</t>
+  </si>
+  <si>
+    <t>Top-down approach does not only work when writing codes but also works when reviewing a system of concepts. Start from a higher level to obtain a genaral structure of this class, to much details of how each module is related to each other.</t>
+  </si>
+  <si>
+    <t>feel more prepared about this midterm</t>
   </si>
 </sst>
 </file>
@@ -765,23 +795,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="216" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="216" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="6" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="6" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="38.1640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.5" style="6" customWidth="1"/>
-    <col min="6" max="6" width="39.33203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="34.6640625" style="6" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="6"/>
+    <col min="1" max="1" width="21.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="39.28515625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="34.7109375" style="6" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -792,7 +822,7 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -801,7 +831,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -810,7 +840,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
@@ -823,7 +853,7 @@
       <c r="F4" s="7"/>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
@@ -836,7 +866,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
@@ -849,7 +879,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -858,7 +888,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -867,7 +897,7 @@
       <c r="F8" s="11"/>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -890,7 +920,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>43839</v>
       </c>
@@ -913,7 +943,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>43842</v>
       </c>
@@ -936,7 +966,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>43846</v>
       </c>
@@ -959,7 +989,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>43850</v>
       </c>
@@ -982,7 +1012,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="144" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>43853</v>
       </c>
@@ -1005,7 +1035,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="98" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="98.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>43858</v>
       </c>
@@ -1028,7 +1058,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="146" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="146.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>43860</v>
       </c>
@@ -1051,7 +1081,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="146" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="146.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>43863</v>
       </c>
@@ -1074,7 +1104,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>43864</v>
       </c>
@@ -1097,7 +1127,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="128" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="128.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>43866</v>
       </c>
@@ -1120,25 +1150,53 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>43867</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>43870</v>
+      </c>
+      <c r="B21" s="2">
+        <v>44055</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1147,7 +1205,7 @@
       <c r="F22" s="4"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1156,7 +1214,7 @@
       <c r="F23" s="4"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1165,7 +1223,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1174,7 +1232,7 @@
       <c r="F25" s="4"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1183,7 +1241,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1192,7 +1250,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1201,7 +1259,7 @@
       <c r="F28" s="4"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1210,7 +1268,7 @@
       <c r="F29" s="4"/>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1219,7 +1277,7 @@
       <c r="F30" s="4"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1228,7 +1286,7 @@
       <c r="F31" s="4"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1237,7 +1295,7 @@
       <c r="F32" s="4"/>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1246,7 +1304,7 @@
       <c r="F33" s="4"/>
       <c r="G33" s="5"/>
     </row>
-    <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1255,7 +1313,7 @@
       <c r="F34" s="4"/>
       <c r="G34" s="5"/>
     </row>
-    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1264,7 +1322,7 @@
       <c r="F35" s="4"/>
       <c r="G35" s="5"/>
     </row>
-    <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1273,7 +1331,7 @@
       <c r="F36" s="4"/>
       <c r="G36" s="5"/>
     </row>
-    <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1282,7 +1340,7 @@
       <c r="F37" s="4"/>
       <c r="G37" s="5"/>
     </row>
-    <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1291,7 +1349,7 @@
       <c r="F38" s="4"/>
       <c r="G38" s="5"/>
     </row>
-    <row r="39" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1300,7 +1358,7 @@
       <c r="F39" s="4"/>
       <c r="G39" s="5"/>
     </row>
-    <row r="40" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1309,7 +1367,7 @@
       <c r="F40" s="4"/>
       <c r="G40" s="5"/>
     </row>
-    <row r="41" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1318,7 +1376,7 @@
       <c r="F41" s="4"/>
       <c r="G41" s="5"/>
     </row>
-    <row r="42" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1327,7 +1385,7 @@
       <c r="F42" s="4"/>
       <c r="G42" s="5"/>
     </row>
-    <row r="43" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -1336,7 +1394,7 @@
       <c r="F43" s="4"/>
       <c r="G43" s="5"/>
     </row>
-    <row r="44" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -1345,7 +1403,7 @@
       <c r="F44" s="4"/>
       <c r="G44" s="5"/>
     </row>
-    <row r="45" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -1354,7 +1412,7 @@
       <c r="F45" s="4"/>
       <c r="G45" s="5"/>
     </row>
-    <row r="46" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -1363,7 +1421,7 @@
       <c r="F46" s="4"/>
       <c r="G46" s="5"/>
     </row>
-    <row r="47" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -1372,7 +1430,7 @@
       <c r="F47" s="4"/>
       <c r="G47" s="5"/>
     </row>
-    <row r="48" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -1381,7 +1439,7 @@
       <c r="F48" s="4"/>
       <c r="G48" s="5"/>
     </row>
-    <row r="49" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -1390,7 +1448,7 @@
       <c r="F49" s="4"/>
       <c r="G49" s="5"/>
     </row>
-    <row r="50" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -1399,7 +1457,7 @@
       <c r="F50" s="4"/>
       <c r="G50" s="5"/>
     </row>
-    <row r="51" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -1408,7 +1466,7 @@
       <c r="F51" s="4"/>
       <c r="G51" s="5"/>
     </row>
-    <row r="52" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -1417,7 +1475,7 @@
       <c r="F52" s="4"/>
       <c r="G52" s="5"/>
     </row>
-    <row r="53" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -1426,7 +1484,7 @@
       <c r="F53" s="4"/>
       <c r="G53" s="5"/>
     </row>
-    <row r="54" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -1435,7 +1493,7 @@
       <c r="F54" s="4"/>
       <c r="G54" s="5"/>
     </row>
-    <row r="55" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -1444,7 +1502,7 @@
       <c r="F55" s="4"/>
       <c r="G55" s="5"/>
     </row>
-    <row r="56" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -1453,7 +1511,7 @@
       <c r="F56" s="4"/>
       <c r="G56" s="5"/>
     </row>
-    <row r="57" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -1462,7 +1520,7 @@
       <c r="F57" s="4"/>
       <c r="G57" s="5"/>
     </row>
-    <row r="58" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -1471,7 +1529,7 @@
       <c r="F58" s="4"/>
       <c r="G58" s="5"/>
     </row>
-    <row r="59" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -1480,7 +1538,7 @@
       <c r="F59" s="4"/>
       <c r="G59" s="5"/>
     </row>
-    <row r="60" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -1489,7 +1547,7 @@
       <c r="F60" s="4"/>
       <c r="G60" s="5"/>
     </row>
-    <row r="61" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -1498,7 +1556,7 @@
       <c r="F61" s="4"/>
       <c r="G61" s="5"/>
     </row>
-    <row r="62" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -1507,7 +1565,7 @@
       <c r="F62" s="4"/>
       <c r="G62" s="5"/>
     </row>
-    <row r="63" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -1516,7 +1574,7 @@
       <c r="F63" s="4"/>
       <c r="G63" s="5"/>
     </row>
-    <row r="64" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -1525,7 +1583,7 @@
       <c r="F64" s="4"/>
       <c r="G64" s="5"/>
     </row>
-    <row r="65" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -1534,7 +1592,7 @@
       <c r="F65" s="4"/>
       <c r="G65" s="5"/>
     </row>
-    <row r="66" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -1543,7 +1601,7 @@
       <c r="F66" s="4"/>
       <c r="G66" s="5"/>
     </row>
-    <row r="67" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -1552,7 +1610,7 @@
       <c r="F67" s="4"/>
       <c r="G67" s="5"/>
     </row>
-    <row r="68" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -1561,7 +1619,7 @@
       <c r="F68" s="4"/>
       <c r="G68" s="5"/>
     </row>
-    <row r="69" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -1570,7 +1628,7 @@
       <c r="F69" s="4"/>
       <c r="G69" s="5"/>
     </row>
-    <row r="70" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -1579,7 +1637,7 @@
       <c r="F70" s="4"/>
       <c r="G70" s="5"/>
     </row>
-    <row r="71" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -1588,7 +1646,7 @@
       <c r="F71" s="4"/>
       <c r="G71" s="5"/>
     </row>
-    <row r="72" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -1597,7 +1655,7 @@
       <c r="F72" s="4"/>
       <c r="G72" s="5"/>
     </row>
-    <row r="73" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -1606,7 +1664,7 @@
       <c r="F73" s="4"/>
       <c r="G73" s="5"/>
     </row>
-    <row r="74" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -1615,7 +1673,7 @@
       <c r="F74" s="4"/>
       <c r="G74" s="5"/>
     </row>
-    <row r="75" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -1624,7 +1682,7 @@
       <c r="F75" s="4"/>
       <c r="G75" s="5"/>
     </row>
-    <row r="76" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -1633,7 +1691,7 @@
       <c r="F76" s="4"/>
       <c r="G76" s="5"/>
     </row>
-    <row r="77" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -1642,7 +1700,7 @@
       <c r="F77" s="4"/>
       <c r="G77" s="5"/>
     </row>
-    <row r="78" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -1651,7 +1709,7 @@
       <c r="F78" s="4"/>
       <c r="G78" s="5"/>
     </row>
-    <row r="79" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -1660,7 +1718,7 @@
       <c r="F79" s="4"/>
       <c r="G79" s="5"/>
     </row>
-    <row r="80" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -1669,7 +1727,7 @@
       <c r="F80" s="4"/>
       <c r="G80" s="5"/>
     </row>
-    <row r="81" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
@@ -1678,7 +1736,7 @@
       <c r="F81" s="4"/>
       <c r="G81" s="5"/>
     </row>
-    <row r="82" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
@@ -1687,7 +1745,7 @@
       <c r="F82" s="4"/>
       <c r="G82" s="5"/>
     </row>
-    <row r="83" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
@@ -1696,7 +1754,7 @@
       <c r="F83" s="4"/>
       <c r="G83" s="5"/>
     </row>
-    <row r="84" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -1705,7 +1763,7 @@
       <c r="F84" s="4"/>
       <c r="G84" s="5"/>
     </row>
-    <row r="85" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -1714,7 +1772,7 @@
       <c r="F85" s="4"/>
       <c r="G85" s="5"/>
     </row>
-    <row r="86" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -1723,7 +1781,7 @@
       <c r="F86" s="4"/>
       <c r="G86" s="5"/>
     </row>
-    <row r="87" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -1732,7 +1790,7 @@
       <c r="F87" s="4"/>
       <c r="G87" s="5"/>
     </row>
-    <row r="88" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
@@ -1741,7 +1799,7 @@
       <c r="F88" s="4"/>
       <c r="G88" s="5"/>
     </row>
-    <row r="89" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
@@ -1750,7 +1808,7 @@
       <c r="F89" s="4"/>
       <c r="G89" s="5"/>
     </row>
-    <row r="90" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -1759,7 +1817,7 @@
       <c r="F90" s="4"/>
       <c r="G90" s="5"/>
     </row>
-    <row r="91" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
@@ -1768,7 +1826,7 @@
       <c r="F91" s="4"/>
       <c r="G91" s="5"/>
     </row>
-    <row r="92" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
@@ -1777,7 +1835,7 @@
       <c r="F92" s="4"/>
       <c r="G92" s="5"/>
     </row>
-    <row r="93" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
@@ -1786,7 +1844,7 @@
       <c r="F93" s="4"/>
       <c r="G93" s="5"/>
     </row>
-    <row r="94" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
@@ -1795,7 +1853,7 @@
       <c r="F94" s="4"/>
       <c r="G94" s="5"/>
     </row>
-    <row r="95" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="4"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
@@ -1804,7 +1862,7 @@
       <c r="F95" s="4"/>
       <c r="G95" s="5"/>
     </row>
-    <row r="96" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
@@ -1813,7 +1871,7 @@
       <c r="F96" s="4"/>
       <c r="G96" s="5"/>
     </row>
-    <row r="97" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
@@ -1822,7 +1880,7 @@
       <c r="F97" s="4"/>
       <c r="G97" s="5"/>
     </row>
-    <row r="98" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="4"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
@@ -1831,7 +1889,7 @@
       <c r="F98" s="4"/>
       <c r="G98" s="5"/>
     </row>
-    <row r="99" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
@@ -1840,7 +1898,7 @@
       <c r="F99" s="4"/>
       <c r="G99" s="5"/>
     </row>
-    <row r="100" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
@@ -1849,7 +1907,7 @@
       <c r="F100" s="4"/>
       <c r="G100" s="5"/>
     </row>
-    <row r="101" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
@@ -1858,7 +1916,7 @@
       <c r="F101" s="4"/>
       <c r="G101" s="5"/>
     </row>
-    <row r="102" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="4"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
@@ -1867,7 +1925,7 @@
       <c r="F102" s="4"/>
       <c r="G102" s="5"/>
     </row>
-    <row r="103" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
@@ -1876,7 +1934,7 @@
       <c r="F103" s="4"/>
       <c r="G103" s="5"/>
     </row>
-    <row r="104" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="4"/>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
@@ -1885,7 +1943,7 @@
       <c r="F104" s="4"/>
       <c r="G104" s="5"/>
     </row>
-    <row r="105" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="4"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
@@ -1894,7 +1952,7 @@
       <c r="F105" s="4"/>
       <c r="G105" s="5"/>
     </row>
-    <row r="106" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="4"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
@@ -1903,7 +1961,7 @@
       <c r="F106" s="4"/>
       <c r="G106" s="5"/>
     </row>
-    <row r="107" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
@@ -1912,7 +1970,7 @@
       <c r="F107" s="4"/>
       <c r="G107" s="5"/>
     </row>
-    <row r="108" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="4"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
@@ -1921,7 +1979,7 @@
       <c r="F108" s="4"/>
       <c r="G108" s="5"/>
     </row>
-    <row r="109" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
@@ -1930,7 +1988,7 @@
       <c r="F109" s="4"/>
       <c r="G109" s="5"/>
     </row>
-    <row r="110" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="4"/>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
@@ -1939,7 +1997,7 @@
       <c r="F110" s="4"/>
       <c r="G110" s="5"/>
     </row>
-    <row r="111" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
@@ -1948,7 +2006,7 @@
       <c r="F111" s="4"/>
       <c r="G111" s="5"/>
     </row>
-    <row r="112" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
@@ -1957,7 +2015,7 @@
       <c r="F112" s="4"/>
       <c r="G112" s="5"/>
     </row>
-    <row r="113" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
@@ -1966,7 +2024,7 @@
       <c r="F113" s="4"/>
       <c r="G113" s="5"/>
     </row>
-    <row r="114" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
@@ -1975,7 +2033,7 @@
       <c r="F114" s="4"/>
       <c r="G114" s="5"/>
     </row>
-    <row r="115" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="13"/>
       <c r="B115" s="13"/>
       <c r="C115" s="13"/>
@@ -1984,7 +2042,7 @@
       <c r="F115" s="13"/>
       <c r="G115" s="14"/>
     </row>
-    <row r="116" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="13"/>
       <c r="B116" s="13"/>
       <c r="C116" s="13"/>
@@ -1993,7 +2051,7 @@
       <c r="F116" s="13"/>
       <c r="G116" s="14"/>
     </row>
-    <row r="117" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="13"/>
       <c r="B117" s="13"/>
       <c r="C117" s="13"/>
@@ -2002,7 +2060,7 @@
       <c r="F117" s="13"/>
       <c r="G117" s="14"/>
     </row>
-    <row r="118" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="13"/>
       <c r="B118" s="13"/>
       <c r="C118" s="13"/>
@@ -2011,7 +2069,7 @@
       <c r="F118" s="13"/>
       <c r="G118" s="14"/>
     </row>
-    <row r="119" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="13"/>
       <c r="B119" s="13"/>
       <c r="C119" s="13"/>
@@ -2020,7 +2078,7 @@
       <c r="F119" s="13"/>
       <c r="G119" s="14"/>
     </row>
-    <row r="120" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="13"/>
       <c r="B120" s="13"/>
       <c r="C120" s="13"/>
@@ -2029,7 +2087,7 @@
       <c r="F120" s="13"/>
       <c r="G120" s="14"/>
     </row>
-    <row r="121" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="13"/>
       <c r="B121" s="13"/>
       <c r="C121" s="13"/>
@@ -2038,7 +2096,7 @@
       <c r="F121" s="13"/>
       <c r="G121" s="14"/>
     </row>
-    <row r="122" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="13"/>
       <c r="B122" s="13"/>
       <c r="C122" s="13"/>
@@ -2047,7 +2105,7 @@
       <c r="F122" s="13"/>
       <c r="G122" s="14"/>
     </row>
-    <row r="123" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="13"/>
       <c r="B123" s="13"/>
       <c r="C123" s="13"/>
@@ -2056,7 +2114,7 @@
       <c r="F123" s="13"/>
       <c r="G123" s="14"/>
     </row>
-    <row r="124" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="13"/>
       <c r="B124" s="13"/>
       <c r="C124" s="13"/>
@@ -2065,7 +2123,7 @@
       <c r="F124" s="13"/>
       <c r="G124" s="14"/>
     </row>
-    <row r="125" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="13"/>
       <c r="B125" s="13"/>
       <c r="C125" s="13"/>

</xml_diff>

<commit_message>
2-20 diary updated (#370)
</commit_message>
<xml_diff>
--- a/diaries/diary-weihuan-fu.xlsx
+++ b/diaries/diary-weihuan-fu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\W2020\diaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weihuanfu/Desktop/SWE-265P/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8B97EF-F55E-48E0-A6FA-9CD2A599FFA3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E80D5E-90F2-9C43-B7D6-6372B1CB8E7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="88">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -275,6 +275,40 @@
   </si>
   <si>
     <t>feel more prepared about this midterm</t>
+  </si>
+  <si>
+    <t>6:30 - 10:30</t>
+  </si>
+  <si>
+    <t>classmates</t>
+  </si>
+  <si>
+    <t>review last lecture contents, get feedback from last homework, learn new stuff</t>
+  </si>
+  <si>
+    <t>learned more key expert practices, some ways of getting a higher level of abstractions of a system and some strategies of how code review works.</t>
+  </si>
+  <si>
+    <t>There are no simple plug-ins that can visualize an architecture pattern of a system, but there are other ways such as grouping source code and communications together based on folders.</t>
+  </si>
+  <si>
+    <t>feel terrified about having to document the architecture of Cassandra and other pieces of the homework</t>
+  </si>
+  <si>
+    <t>13:00 - 15:00</t>
+  </si>
+  <si>
+    <t>do homework 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Looked up stakeholders of Cassandra, essential functional and non-functional aspects of the system. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">It was not too hard to find stakeholders of Cassandra as it is a pretty well-known open source project. What interesting is that not just big companies are using it, even individual and some small businesses are using it as well.
+</t>
+  </si>
+  <si>
+    <t>feel accompolished after finishing most of the homework</t>
   </si>
 </sst>
 </file>
@@ -793,25 +827,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
-  <dimension ref="A1:G125"/>
+  <dimension ref="A1:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="216" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="216" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="38.140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="39.28515625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="34.7109375" style="6" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="21.5" style="6" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="6" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="38.1640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.5" style="6" customWidth="1"/>
+    <col min="6" max="6" width="39.33203125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="34.6640625" style="6" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -822,7 +856,7 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -831,7 +865,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -840,7 +874,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
@@ -853,7 +887,7 @@
       <c r="F4" s="7"/>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
@@ -866,7 +900,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
@@ -879,7 +913,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -888,7 +922,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -897,7 +931,7 @@
       <c r="F8" s="11"/>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -920,7 +954,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>43839</v>
       </c>
@@ -943,7 +977,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>43842</v>
       </c>
@@ -966,7 +1000,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="136" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>43846</v>
       </c>
@@ -989,7 +1023,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>43850</v>
       </c>
@@ -1012,7 +1046,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="144" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>43853</v>
       </c>
@@ -1035,7 +1069,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="98.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>43858</v>
       </c>
@@ -1058,7 +1092,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="146.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="146" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>43860</v>
       </c>
@@ -1081,7 +1115,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="146.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="146" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>43863</v>
       </c>
@@ -1104,7 +1138,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>43864</v>
       </c>
@@ -1127,7 +1161,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="128.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="128" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>43866</v>
       </c>
@@ -1150,7 +1184,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="149.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>43867</v>
       </c>
@@ -1173,12 +1207,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>43870</v>
       </c>
-      <c r="B21" s="2">
-        <v>44055</v>
+      <c r="B21" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>72</v>
@@ -1196,25 +1230,53 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>43877</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="119" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>43881</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="101" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1223,7 +1285,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1232,7 +1294,7 @@
       <c r="F25" s="4"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1241,7 +1303,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1250,7 +1312,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1259,7 +1321,7 @@
       <c r="F28" s="4"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1268,7 +1330,7 @@
       <c r="F29" s="4"/>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1277,7 +1339,7 @@
       <c r="F30" s="4"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1286,7 +1348,7 @@
       <c r="F31" s="4"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1295,7 +1357,7 @@
       <c r="F32" s="4"/>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1304,7 +1366,7 @@
       <c r="F33" s="4"/>
       <c r="G33" s="5"/>
     </row>
-    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1313,7 +1375,7 @@
       <c r="F34" s="4"/>
       <c r="G34" s="5"/>
     </row>
-    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1322,7 +1384,7 @@
       <c r="F35" s="4"/>
       <c r="G35" s="5"/>
     </row>
-    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1331,7 +1393,7 @@
       <c r="F36" s="4"/>
       <c r="G36" s="5"/>
     </row>
-    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1340,7 +1402,7 @@
       <c r="F37" s="4"/>
       <c r="G37" s="5"/>
     </row>
-    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1349,7 +1411,7 @@
       <c r="F38" s="4"/>
       <c r="G38" s="5"/>
     </row>
-    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1358,7 +1420,7 @@
       <c r="F39" s="4"/>
       <c r="G39" s="5"/>
     </row>
-    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1367,7 +1429,7 @@
       <c r="F40" s="4"/>
       <c r="G40" s="5"/>
     </row>
-    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1376,7 +1438,7 @@
       <c r="F41" s="4"/>
       <c r="G41" s="5"/>
     </row>
-    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1385,7 +1447,7 @@
       <c r="F42" s="4"/>
       <c r="G42" s="5"/>
     </row>
-    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -1394,7 +1456,7 @@
       <c r="F43" s="4"/>
       <c r="G43" s="5"/>
     </row>
-    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -1403,7 +1465,7 @@
       <c r="F44" s="4"/>
       <c r="G44" s="5"/>
     </row>
-    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -1412,7 +1474,7 @@
       <c r="F45" s="4"/>
       <c r="G45" s="5"/>
     </row>
-    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -1421,7 +1483,7 @@
       <c r="F46" s="4"/>
       <c r="G46" s="5"/>
     </row>
-    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -1430,7 +1492,7 @@
       <c r="F47" s="4"/>
       <c r="G47" s="5"/>
     </row>
-    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -1439,7 +1501,7 @@
       <c r="F48" s="4"/>
       <c r="G48" s="5"/>
     </row>
-    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -1448,7 +1510,7 @@
       <c r="F49" s="4"/>
       <c r="G49" s="5"/>
     </row>
-    <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -1457,7 +1519,7 @@
       <c r="F50" s="4"/>
       <c r="G50" s="5"/>
     </row>
-    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -1466,7 +1528,7 @@
       <c r="F51" s="4"/>
       <c r="G51" s="5"/>
     </row>
-    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -1475,7 +1537,7 @@
       <c r="F52" s="4"/>
       <c r="G52" s="5"/>
     </row>
-    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -1484,7 +1546,7 @@
       <c r="F53" s="4"/>
       <c r="G53" s="5"/>
     </row>
-    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -1493,7 +1555,7 @@
       <c r="F54" s="4"/>
       <c r="G54" s="5"/>
     </row>
-    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -1502,7 +1564,7 @@
       <c r="F55" s="4"/>
       <c r="G55" s="5"/>
     </row>
-    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -1511,7 +1573,7 @@
       <c r="F56" s="4"/>
       <c r="G56" s="5"/>
     </row>
-    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -1520,7 +1582,7 @@
       <c r="F57" s="4"/>
       <c r="G57" s="5"/>
     </row>
-    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -1529,7 +1591,7 @@
       <c r="F58" s="4"/>
       <c r="G58" s="5"/>
     </row>
-    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -1538,7 +1600,7 @@
       <c r="F59" s="4"/>
       <c r="G59" s="5"/>
     </row>
-    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -1547,7 +1609,7 @@
       <c r="F60" s="4"/>
       <c r="G60" s="5"/>
     </row>
-    <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -1556,7 +1618,7 @@
       <c r="F61" s="4"/>
       <c r="G61" s="5"/>
     </row>
-    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -1565,7 +1627,7 @@
       <c r="F62" s="4"/>
       <c r="G62" s="5"/>
     </row>
-    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -1574,7 +1636,7 @@
       <c r="F63" s="4"/>
       <c r="G63" s="5"/>
     </row>
-    <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -1583,7 +1645,7 @@
       <c r="F64" s="4"/>
       <c r="G64" s="5"/>
     </row>
-    <row r="65" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -1592,7 +1654,7 @@
       <c r="F65" s="4"/>
       <c r="G65" s="5"/>
     </row>
-    <row r="66" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -1601,7 +1663,7 @@
       <c r="F66" s="4"/>
       <c r="G66" s="5"/>
     </row>
-    <row r="67" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -1610,7 +1672,7 @@
       <c r="F67" s="4"/>
       <c r="G67" s="5"/>
     </row>
-    <row r="68" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -1619,7 +1681,7 @@
       <c r="F68" s="4"/>
       <c r="G68" s="5"/>
     </row>
-    <row r="69" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -1628,7 +1690,7 @@
       <c r="F69" s="4"/>
       <c r="G69" s="5"/>
     </row>
-    <row r="70" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -1637,7 +1699,7 @@
       <c r="F70" s="4"/>
       <c r="G70" s="5"/>
     </row>
-    <row r="71" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -1646,7 +1708,7 @@
       <c r="F71" s="4"/>
       <c r="G71" s="5"/>
     </row>
-    <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -1655,7 +1717,7 @@
       <c r="F72" s="4"/>
       <c r="G72" s="5"/>
     </row>
-    <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -1664,7 +1726,7 @@
       <c r="F73" s="4"/>
       <c r="G73" s="5"/>
     </row>
-    <row r="74" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -1673,7 +1735,7 @@
       <c r="F74" s="4"/>
       <c r="G74" s="5"/>
     </row>
-    <row r="75" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -1682,7 +1744,7 @@
       <c r="F75" s="4"/>
       <c r="G75" s="5"/>
     </row>
-    <row r="76" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -1691,7 +1753,7 @@
       <c r="F76" s="4"/>
       <c r="G76" s="5"/>
     </row>
-    <row r="77" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -1700,7 +1762,7 @@
       <c r="F77" s="4"/>
       <c r="G77" s="5"/>
     </row>
-    <row r="78" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -1709,7 +1771,7 @@
       <c r="F78" s="4"/>
       <c r="G78" s="5"/>
     </row>
-    <row r="79" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -1718,7 +1780,7 @@
       <c r="F79" s="4"/>
       <c r="G79" s="5"/>
     </row>
-    <row r="80" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -1727,7 +1789,7 @@
       <c r="F80" s="4"/>
       <c r="G80" s="5"/>
     </row>
-    <row r="81" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
@@ -1736,7 +1798,7 @@
       <c r="F81" s="4"/>
       <c r="G81" s="5"/>
     </row>
-    <row r="82" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
@@ -1745,7 +1807,7 @@
       <c r="F82" s="4"/>
       <c r="G82" s="5"/>
     </row>
-    <row r="83" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
@@ -1754,7 +1816,7 @@
       <c r="F83" s="4"/>
       <c r="G83" s="5"/>
     </row>
-    <row r="84" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -1763,7 +1825,7 @@
       <c r="F84" s="4"/>
       <c r="G84" s="5"/>
     </row>
-    <row r="85" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -1772,7 +1834,7 @@
       <c r="F85" s="4"/>
       <c r="G85" s="5"/>
     </row>
-    <row r="86" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -1781,7 +1843,7 @@
       <c r="F86" s="4"/>
       <c r="G86" s="5"/>
     </row>
-    <row r="87" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -1790,7 +1852,7 @@
       <c r="F87" s="4"/>
       <c r="G87" s="5"/>
     </row>
-    <row r="88" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
@@ -1799,7 +1861,7 @@
       <c r="F88" s="4"/>
       <c r="G88" s="5"/>
     </row>
-    <row r="89" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
@@ -1808,7 +1870,7 @@
       <c r="F89" s="4"/>
       <c r="G89" s="5"/>
     </row>
-    <row r="90" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -1817,7 +1879,7 @@
       <c r="F90" s="4"/>
       <c r="G90" s="5"/>
     </row>
-    <row r="91" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
@@ -1826,7 +1888,7 @@
       <c r="F91" s="4"/>
       <c r="G91" s="5"/>
     </row>
-    <row r="92" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
@@ -1835,7 +1897,7 @@
       <c r="F92" s="4"/>
       <c r="G92" s="5"/>
     </row>
-    <row r="93" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
@@ -1844,7 +1906,7 @@
       <c r="F93" s="4"/>
       <c r="G93" s="5"/>
     </row>
-    <row r="94" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
@@ -1853,7 +1915,7 @@
       <c r="F94" s="4"/>
       <c r="G94" s="5"/>
     </row>
-    <row r="95" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="4"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
@@ -1862,7 +1924,7 @@
       <c r="F95" s="4"/>
       <c r="G95" s="5"/>
     </row>
-    <row r="96" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="4"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
@@ -1871,7 +1933,7 @@
       <c r="F96" s="4"/>
       <c r="G96" s="5"/>
     </row>
-    <row r="97" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="4"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
@@ -1880,7 +1942,7 @@
       <c r="F97" s="4"/>
       <c r="G97" s="5"/>
     </row>
-    <row r="98" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="4"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
@@ -1889,7 +1951,7 @@
       <c r="F98" s="4"/>
       <c r="G98" s="5"/>
     </row>
-    <row r="99" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="4"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
@@ -1898,7 +1960,7 @@
       <c r="F99" s="4"/>
       <c r="G99" s="5"/>
     </row>
-    <row r="100" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
@@ -1907,7 +1969,7 @@
       <c r="F100" s="4"/>
       <c r="G100" s="5"/>
     </row>
-    <row r="101" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="4"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
@@ -1916,7 +1978,7 @@
       <c r="F101" s="4"/>
       <c r="G101" s="5"/>
     </row>
-    <row r="102" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="4"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
@@ -1925,7 +1987,7 @@
       <c r="F102" s="4"/>
       <c r="G102" s="5"/>
     </row>
-    <row r="103" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
@@ -1934,7 +1996,7 @@
       <c r="F103" s="4"/>
       <c r="G103" s="5"/>
     </row>
-    <row r="104" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="4"/>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
@@ -1943,7 +2005,7 @@
       <c r="F104" s="4"/>
       <c r="G104" s="5"/>
     </row>
-    <row r="105" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="4"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
@@ -1952,7 +2014,7 @@
       <c r="F105" s="4"/>
       <c r="G105" s="5"/>
     </row>
-    <row r="106" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="4"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
@@ -1961,7 +2023,7 @@
       <c r="F106" s="4"/>
       <c r="G106" s="5"/>
     </row>
-    <row r="107" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
@@ -1970,7 +2032,7 @@
       <c r="F107" s="4"/>
       <c r="G107" s="5"/>
     </row>
-    <row r="108" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="4"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
@@ -1979,7 +2041,7 @@
       <c r="F108" s="4"/>
       <c r="G108" s="5"/>
     </row>
-    <row r="109" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
@@ -1988,7 +2050,7 @@
       <c r="F109" s="4"/>
       <c r="G109" s="5"/>
     </row>
-    <row r="110" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="4"/>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
@@ -1997,7 +2059,7 @@
       <c r="F110" s="4"/>
       <c r="G110" s="5"/>
     </row>
-    <row r="111" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
@@ -2006,7 +2068,7 @@
       <c r="F111" s="4"/>
       <c r="G111" s="5"/>
     </row>
-    <row r="112" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
@@ -2015,7 +2077,7 @@
       <c r="F112" s="4"/>
       <c r="G112" s="5"/>
     </row>
-    <row r="113" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
@@ -2024,7 +2086,7 @@
       <c r="F113" s="4"/>
       <c r="G113" s="5"/>
     </row>
-    <row r="114" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
@@ -2033,16 +2095,16 @@
       <c r="F114" s="4"/>
       <c r="G114" s="5"/>
     </row>
-    <row r="115" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A115" s="13"/>
-      <c r="B115" s="13"/>
-      <c r="C115" s="13"/>
-      <c r="D115" s="13"/>
-      <c r="E115" s="13"/>
-      <c r="F115" s="13"/>
-      <c r="G115" s="14"/>
-    </row>
-    <row r="116" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A115" s="4"/>
+      <c r="B115" s="4"/>
+      <c r="C115" s="4"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="4"/>
+      <c r="F115" s="4"/>
+      <c r="G115" s="5"/>
+    </row>
+    <row r="116" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="13"/>
       <c r="B116" s="13"/>
       <c r="C116" s="13"/>
@@ -2051,7 +2113,7 @@
       <c r="F116" s="13"/>
       <c r="G116" s="14"/>
     </row>
-    <row r="117" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="13"/>
       <c r="B117" s="13"/>
       <c r="C117" s="13"/>
@@ -2060,7 +2122,7 @@
       <c r="F117" s="13"/>
       <c r="G117" s="14"/>
     </row>
-    <row r="118" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="13"/>
       <c r="B118" s="13"/>
       <c r="C118" s="13"/>
@@ -2069,7 +2131,7 @@
       <c r="F118" s="13"/>
       <c r="G118" s="14"/>
     </row>
-    <row r="119" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="13"/>
       <c r="B119" s="13"/>
       <c r="C119" s="13"/>
@@ -2078,7 +2140,7 @@
       <c r="F119" s="13"/>
       <c r="G119" s="14"/>
     </row>
-    <row r="120" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="13"/>
       <c r="B120" s="13"/>
       <c r="C120" s="13"/>
@@ -2087,7 +2149,7 @@
       <c r="F120" s="13"/>
       <c r="G120" s="14"/>
     </row>
-    <row r="121" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="13"/>
       <c r="B121" s="13"/>
       <c r="C121" s="13"/>
@@ -2096,7 +2158,7 @@
       <c r="F121" s="13"/>
       <c r="G121" s="14"/>
     </row>
-    <row r="122" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="13"/>
       <c r="B122" s="13"/>
       <c r="C122" s="13"/>
@@ -2105,7 +2167,7 @@
       <c r="F122" s="13"/>
       <c r="G122" s="14"/>
     </row>
-    <row r="123" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="13"/>
       <c r="B123" s="13"/>
       <c r="C123" s="13"/>
@@ -2114,7 +2176,7 @@
       <c r="F123" s="13"/>
       <c r="G123" s="14"/>
     </row>
-    <row r="124" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="13"/>
       <c r="B124" s="13"/>
       <c r="C124" s="13"/>
@@ -2123,7 +2185,7 @@
       <c r="F124" s="13"/>
       <c r="G124" s="14"/>
     </row>
-    <row r="125" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="13"/>
       <c r="B125" s="13"/>
       <c r="C125" s="13"/>
@@ -2131,6 +2193,15 @@
       <c r="E125" s="13"/>
       <c r="F125" s="13"/>
       <c r="G125" s="14"/>
+    </row>
+    <row r="126" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A126" s="13"/>
+      <c r="B126" s="13"/>
+      <c r="C126" s="13"/>
+      <c r="D126" s="13"/>
+      <c r="E126" s="13"/>
+      <c r="F126" s="13"/>
+      <c r="G126" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
3/2 diaries updated --Weihuan Fu
</commit_message>
<xml_diff>
--- a/diaries/diary-weihuan-fu.xlsx
+++ b/diaries/diary-weihuan-fu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weihuanfu/Desktop/SWE-265P/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E80D5E-90F2-9C43-B7D6-6372B1CB8E7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C165712E-0974-6148-B644-AE00BC3CD8B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="116">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -309,6 +309,90 @@
   </si>
   <si>
     <t>feel accompolished after finishing most of the homework</t>
+  </si>
+  <si>
+    <t>12:30 - 3:00</t>
+  </si>
+  <si>
+    <t>Going through social context of Cassandra and read about pull request for homework</t>
+  </si>
+  <si>
+    <t>Discovered general social context, 3 interesting pull requests and understood how a normal pull request work</t>
+  </si>
+  <si>
+    <t>It was interesting to discover how people try to contribute to big open source project and how the contributor communicate with reviewers frequently concerning any related problems to the pull request.</t>
+  </si>
+  <si>
+    <t>Almost every open source project has a standard of creating a pull request and getting merged, especially Cassandra. However, since Cassandra is a very big and integrate system, the change of getting merged by the developer is almost zero from its pull request history. Among reasons of rejections, a lot of them is because of coding standard. This taught me how important it is to have a good coding habit and create meaningful and consisitent variable names, etc.</t>
+  </si>
+  <si>
+    <t>Finish the other 2 interesting pull requests and start to write about interesting issues.</t>
+  </si>
+  <si>
+    <t>Finished all interesting pull requests and 5 interesting issues.</t>
+  </si>
+  <si>
+    <t>Reading people's comments under issues was very helpful to me to understand the cycle of from detecting a bug to possibly fixing it. I understood that even for well-known project like Cassandra, which has been used widely in the industry, there are a lot existing issues and improvements that either developers or contributors are working on. Also the fact that most of the issues remain open even after several years taught me how time-comsuming and difficult it is to fix some issues.</t>
+  </si>
+  <si>
+    <t>Satisfied to finish homework and explore current active open issues.</t>
+  </si>
+  <si>
+    <t>15:00 - 17:00</t>
+  </si>
+  <si>
+    <t>Help discover architectural design of Cassandra and verify if it is implemented as the source code</t>
+  </si>
+  <si>
+    <t>By using some tools learned from class and searching about articles online, we were able to generalize the architecture structure of Cassandra and match that with the source code</t>
+  </si>
+  <si>
+    <t>Since Cassandra is a pretty active open source project, the articles that was posted online some time ago probably does not match what it is now. We understood the difference might exist and applied some strategies to generalize structure and detect difference. Lesson learned was that never assume the structure is exactly implemented as it is based on 3rd party articles or even documents from its own developers (as it might be out-dated)</t>
+  </si>
+  <si>
+    <t>Losed at first when trying to verify structure but felt better after breaking down the problem.</t>
+  </si>
+  <si>
+    <t>Learn more about key expert practices and some design patterns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learned about Strategy Pattern with a concrete examplea walked through. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design pattern is something that I really want to learn a long time ago because this is really helpful for me to write elegant and efficient codes instead of messy ones. </t>
+  </si>
+  <si>
+    <t>Very excited to learn about some design patterns and ready to learn more patterns</t>
+  </si>
+  <si>
+    <t>18:00 - 21:00</t>
+  </si>
+  <si>
+    <t>Discover more about strategy patterns</t>
+  </si>
+  <si>
+    <t>Watched Youtube video provided in the lecture slide to learn more about strategy patterns and wrote a Java example myself to practice my understanding about this pattern</t>
+  </si>
+  <si>
+    <t>By learning about why such pattern exist and what problems does this pattern solve, I understand more about object-oriented design. It was also very helpful that instead of just watching people explaining a pattern, I wrote an example myself for deeper understanding</t>
+  </si>
+  <si>
+    <t>Feel good about being able to following the examples and write a implementation of such pattern myself. Hopefully I will be able to use this pattern when coding up my projects</t>
+  </si>
+  <si>
+    <t>12:30 - 16:00</t>
+  </si>
+  <si>
+    <t>Discover more design patterns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Watched videos and read articles about factory method pattern. Wrote an example myself that implements this pattern </t>
+  </si>
+  <si>
+    <t>A lot of this patterns aims to eliminate duplicate codes and increase flexibility and efficiency of the system. It was not too hard to follow along and write a simple example, but it takes more effort to fully understand them and use them in my own projects</t>
+  </si>
+  <si>
+    <t>Amazed by how elegant those design patterns are and ready to learn more about it</t>
   </si>
 </sst>
 </file>
@@ -829,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="216" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1276,59 +1360,143 @@
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="101" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="5"/>
-    </row>
-    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="5"/>
-    </row>
-    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="5"/>
-    </row>
-    <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="5"/>
+    <row r="24" spans="1:7" ht="176" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>43883</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="227" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>43885</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="177" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>43887</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>43888</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="122" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>43891</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>43893</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>

</xml_diff>